<commit_message>
Relazione 95% e risultati
Relazione 95% e risultati
</commit_message>
<xml_diff>
--- a/Risultati.xlsx
+++ b/Risultati.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2740ff5e8d6d8ebd/Documenti/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emilio Casella\OneDrive\Documenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{5FD730AC-8776-451C-B3FC-6FE612676AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4B6EACE1-EEA4-468E-BBAC-0BCC0954E5CD}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="8_{5FD730AC-8776-451C-B3FC-6FE612676AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23DBACC2-2C62-458D-8B2E-27D22DE2D783}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="20">
   <si>
     <t>RI</t>
   </si>
   <si>
     <t>AUC</t>
-  </si>
-  <si>
-    <t>F1</t>
   </si>
   <si>
     <t>Tabella N2VVSKMeans</t>
@@ -405,28 +402,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -434,11 +428,8 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J2" t="s">
         <v>0</v>
@@ -447,12 +438,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>0.66</v>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
       <c r="C3">
         <v>4.0000000000000001E-3</v>
@@ -463,28 +451,22 @@
       <c r="E3">
         <v>0.49</v>
       </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>0.76</v>
+      <c r="H3" t="s">
+        <v>3</v>
       </c>
       <c r="I3">
         <v>1E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3">
         <v>0.51</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.59</v>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
       <c r="C4">
         <v>2.9999999999999997E-4</v>
@@ -495,11 +477,8 @@
       <c r="E4">
         <v>0.5</v>
       </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>0.7</v>
+      <c r="H4" t="s">
+        <v>4</v>
       </c>
       <c r="I4">
         <v>1E-3</v>
@@ -511,12 +490,9 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.55000000000000004</v>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>5</v>
       </c>
       <c r="C5">
         <v>3.0000000000000001E-3</v>
@@ -527,11 +503,8 @@
       <c r="E5">
         <v>0.50700000000000001</v>
       </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>0.59</v>
+      <c r="H5" t="s">
+        <v>5</v>
       </c>
       <c r="I5">
         <v>8.9999999999999998E-4</v>
@@ -543,12 +516,9 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0.31</v>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
       <c r="C6">
         <v>3.0000000000000001E-3</v>
@@ -559,11 +529,8 @@
       <c r="E6">
         <v>0.5</v>
       </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <v>0.55000000000000004</v>
+      <c r="H6" t="s">
+        <v>6</v>
       </c>
       <c r="I6">
         <v>1.1000000000000001E-3</v>
@@ -575,20 +542,17 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -596,11 +560,8 @@
       <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
-        <v>2</v>
-      </c>
       <c r="I11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J11" t="s">
         <v>0</v>
@@ -609,12 +570,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>0.71</v>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>10</v>
       </c>
       <c r="C12">
         <v>0.36</v>
@@ -625,11 +583,8 @@
       <c r="E12">
         <v>0.85</v>
       </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12">
-        <v>0.69</v>
+      <c r="H12" t="s">
+        <v>10</v>
       </c>
       <c r="I12">
         <v>0.12</v>
@@ -641,12 +596,9 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0.69</v>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>11</v>
       </c>
       <c r="C13">
         <v>0.38</v>
@@ -657,11 +609,8 @@
       <c r="E13">
         <v>0.87</v>
       </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13">
-        <v>0.62</v>
+      <c r="H13" t="s">
+        <v>11</v>
       </c>
       <c r="I13">
         <v>0.12</v>
@@ -673,12 +622,9 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0.4</v>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>12</v>
       </c>
       <c r="C14">
         <v>0.35</v>
@@ -689,11 +635,8 @@
       <c r="E14">
         <v>0.78</v>
       </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14">
-        <v>0.63</v>
+      <c r="H14" t="s">
+        <v>12</v>
       </c>
       <c r="I14">
         <v>0.12</v>
@@ -705,12 +648,9 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0.38</v>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>13</v>
       </c>
       <c r="C15">
         <v>0.38</v>
@@ -721,11 +661,8 @@
       <c r="E15">
         <v>0.82</v>
       </c>
-      <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15">
-        <v>0.71</v>
+      <c r="H15" t="s">
+        <v>13</v>
       </c>
       <c r="I15">
         <v>0.11</v>
@@ -737,20 +674,17 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
         <v>16</v>
       </c>
-      <c r="H23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
@@ -758,11 +692,8 @@
       <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="H24" t="s">
-        <v>2</v>
-      </c>
       <c r="I24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J24" t="s">
         <v>0</v>
@@ -771,12 +702,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <v>0.44</v>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>3</v>
       </c>
       <c r="C25">
         <v>5.0000000000000001E-3</v>
@@ -787,11 +715,8 @@
       <c r="E25">
         <v>0.6</v>
       </c>
-      <c r="G25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25">
-        <v>0.59</v>
+      <c r="H25" t="s">
+        <v>3</v>
       </c>
       <c r="I25">
         <v>1E-3</v>
@@ -803,12 +728,9 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>0.26</v>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>4</v>
       </c>
       <c r="C26">
         <v>3.0000000000000001E-3</v>
@@ -819,11 +741,8 @@
       <c r="E26">
         <v>0.49</v>
       </c>
-      <c r="G26" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26">
-        <v>0.44</v>
+      <c r="H26" t="s">
+        <v>4</v>
       </c>
       <c r="I26">
         <v>8.9999999999999998E-4</v>
@@ -835,12 +754,9 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27">
-        <v>0.48</v>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>5</v>
       </c>
       <c r="C27">
         <v>3.0000000000000001E-3</v>
@@ -851,11 +767,8 @@
       <c r="E27">
         <v>0.5</v>
       </c>
-      <c r="G27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27">
-        <v>0.28999999999999998</v>
+      <c r="H27" t="s">
+        <v>5</v>
       </c>
       <c r="I27">
         <v>8.0000000000000004E-4</v>
@@ -867,12 +780,9 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28">
-        <v>0.6</v>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>6</v>
       </c>
       <c r="C28">
         <v>2E-3</v>
@@ -883,11 +793,8 @@
       <c r="E28">
         <v>0.48</v>
       </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28">
-        <v>0.23</v>
+      <c r="H28" t="s">
+        <v>6</v>
       </c>
       <c r="I28">
         <v>1E-3</v>
@@ -899,20 +806,17 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
         <v>18</v>
       </c>
-      <c r="H32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
         <v>0</v>
@@ -920,11 +824,8 @@
       <c r="E33" t="s">
         <v>1</v>
       </c>
-      <c r="H33" t="s">
-        <v>2</v>
-      </c>
       <c r="I33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J33" t="s">
         <v>0</v>
@@ -933,12 +834,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34">
-        <v>0.24</v>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>10</v>
       </c>
       <c r="C34">
         <v>0.35</v>
@@ -949,11 +847,8 @@
       <c r="E34">
         <v>0.85</v>
       </c>
-      <c r="G34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34">
-        <v>0.62</v>
+      <c r="H34" t="s">
+        <v>10</v>
       </c>
       <c r="I34">
         <v>0.2</v>
@@ -965,12 +860,9 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35">
-        <v>0.32</v>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>11</v>
       </c>
       <c r="C35">
         <v>0.36</v>
@@ -981,11 +873,8 @@
       <c r="E35">
         <v>0.82</v>
       </c>
-      <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35">
-        <v>0.64</v>
+      <c r="H35" t="s">
+        <v>11</v>
       </c>
       <c r="I35">
         <v>0.19</v>
@@ -997,12 +886,9 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36">
-        <v>0.44</v>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>12</v>
       </c>
       <c r="C36">
         <v>0.37</v>
@@ -1013,11 +899,8 @@
       <c r="E36">
         <v>0.83</v>
       </c>
-      <c r="G36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36">
-        <v>0.56000000000000005</v>
+      <c r="H36" t="s">
+        <v>12</v>
       </c>
       <c r="I36">
         <v>0.11</v>
@@ -1029,12 +912,9 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37">
-        <v>0.72</v>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>13</v>
       </c>
       <c r="C37">
         <v>0.34</v>
@@ -1045,11 +925,8 @@
       <c r="E37">
         <v>0.84</v>
       </c>
-      <c r="G37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37">
-        <v>0.64</v>
+      <c r="H37" t="s">
+        <v>13</v>
       </c>
       <c r="I37">
         <v>0.13</v>

</xml_diff>